<commit_message>
Creating table of model fit
</commit_message>
<xml_diff>
--- a/USA/state/data/dic/1980_2016/DIC comparison pw and nonpw all ages 1980-2016.xlsx
+++ b/USA/state/data/dic/1980_2016/DIC comparison pw and nonpw all ages 1980-2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/mortality/USA/state/data/dic/1980_2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D0C90D-C858-044F-85E8-E656BA7CD134}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FECB84-A90A-4244-990C-17743BC5BC38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1280" windowWidth="23620" windowHeight="15100" xr2:uid="{C5D6F9F6-4735-9542-B608-875F16A3F9AD}"/>
+    <workbookView xWindow="-6900" yWindow="-17940" windowWidth="23620" windowHeight="15100" xr2:uid="{C5D6F9F6-4735-9542-B608-875F16A3F9AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C297E7-6797-2342-9E80-1C39CEF8FE4F}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +484,7 @@
         <v>77421.31</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F21" si="0">IF(D3&lt;E3,"non-pw","pw")</f>
+        <f t="shared" ref="F3:F41" si="0">IF(D3&lt;E3,"non-pw","pw")</f>
         <v>pw</v>
       </c>
     </row>
@@ -975,6 +975,16 @@
       <c r="C31">
         <v>85</v>
       </c>
+      <c r="D31">
+        <v>130685.02</v>
+      </c>
+      <c r="E31">
+        <v>130688.02</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -987,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1009,7 +1019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1031,7 +1041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1042,7 +1052,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1053,7 +1063,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1074,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1074,8 +1084,18 @@
       <c r="C40">
         <v>75</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>135122.01</v>
+      </c>
+      <c r="E40">
+        <v>135126.31</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1084,6 +1104,16 @@
       </c>
       <c r="C41">
         <v>85</v>
+      </c>
+      <c r="D41">
+        <v>142448.32999999999</v>
+      </c>
+      <c r="E41">
+        <v>142452.98000000001</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated age split model
</commit_message>
<xml_diff>
--- a/USA/state/data/dic/1980_2016/DIC comparison pw and nonpw all ages 1980-2016.xlsx
+++ b/USA/state/data/dic/1980_2016/DIC comparison pw and nonpw all ages 1980-2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/mortality/USA/state/data/dic/1980_2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C801C5-86E8-2145-AB4E-89BE25780A2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8755A6B-57DA-054C-B552-850708C40F18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6900" yWindow="-17940" windowWidth="23620" windowHeight="15100" xr2:uid="{C5D6F9F6-4735-9542-B608-875F16A3F9AD}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{C5D6F9F6-4735-9542-B608-875F16A3F9AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C297E7-6797-2342-9E80-1C39CEF8FE4F}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F31" sqref="F30:F31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,6 +942,16 @@
       <c r="C28">
         <v>55</v>
       </c>
+      <c r="D28">
+        <v>120523.83</v>
+      </c>
+      <c r="E28">
+        <v>120528.28</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -953,6 +963,16 @@
       <c r="C29">
         <v>65</v>
       </c>
+      <c r="D29">
+        <v>129515.48</v>
+      </c>
+      <c r="E29">
+        <v>129516.42</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1072,6 +1092,16 @@
       <c r="C38">
         <v>55</v>
       </c>
+      <c r="D38">
+        <v>113458.35</v>
+      </c>
+      <c r="E38">
+        <v>113463.93</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1082,6 +1112,16 @@
       </c>
       <c r="C39">
         <v>65</v>
+      </c>
+      <c r="D39">
+        <v>123525.49</v>
+      </c>
+      <c r="E39">
+        <v>123530.41</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>non-pw</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>